<commit_message>
Update test inputs using 10-14-22 PEARS schema
</commit_message>
<xml_diff>
--- a/tests/test_inputs/FY23_INEP_Staff_List.xlsx
+++ b/tests/test_inputs/FY23_INEP_Staff_List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-25650" yWindow="960" windowWidth="21600" windowHeight="11265" tabRatio="785" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SNAP-Ed Staff List" sheetId="1" state="visible" r:id="rId1"/>
@@ -641,6 +641,21 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -673,21 +688,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -2850,12 +2850,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Jones, Leslie</t>
+          <t>Snyder, Brittany</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Leslie.Jones@fake_domain.com</t>
+          <t>Brittany.Snyder@fake_domain.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2865,12 +2865,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Mccarthy, Roy</t>
+          <t>Rose, Jacob</t>
         </is>
       </c>
     </row>
@@ -2894,12 +2894,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Sanchez, Eric</t>
+          <t>Velez, Dustin</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Eric.Sanchez@fake_domain.com</t>
+          <t>Dustin.Velez@fake_domain.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -2909,12 +2909,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Mccarthy, Roy</t>
+          <t>Rose, Jacob</t>
         </is>
       </c>
     </row>
@@ -2938,12 +2938,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Evans, Melanie</t>
+          <t>Sparks, Bruce</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Melanie.Evans@fake_domain.com</t>
+          <t>Bruce.Sparks@fake_domain.com</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -2953,12 +2953,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Mccarthy, Roy</t>
+          <t>Rose, Jacob</t>
         </is>
       </c>
     </row>
@@ -2982,12 +2982,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Young, Thomas</t>
+          <t>Jones, Robert</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Thomas.Young@fake_domain.com</t>
+          <t>Robert.Jones@fake_domain.com</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -2997,12 +2997,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Mccarthy, Roy</t>
+          <t>Rose, Jacob</t>
         </is>
       </c>
     </row>
@@ -3026,12 +3026,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Jones, Erica</t>
+          <t>Martin, Jesse</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Erica.Jones@fake_domain.com</t>
+          <t>Jesse.Martin@fake_domain.com</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -3041,12 +3041,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Mccarthy, Roy</t>
+          <t>Rose, Jacob</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Simmons, Barbara</t>
+          <t>Barnes, Amy</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Barbara.Simmons@fake_domain.com</t>
+          <t>Amy.Barnes@fake_domain.com</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -3085,12 +3085,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Beck, Johnny</t>
+          <t>Ryan, Amy</t>
         </is>
       </c>
     </row>
@@ -3114,12 +3114,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Mathews, Monica</t>
+          <t>Rodgers, David</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Monica.Mathews@fake_domain.com</t>
+          <t>David.Rodgers@fake_domain.com</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -3129,12 +3129,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Beck, Johnny</t>
+          <t>Ryan, Amy</t>
         </is>
       </c>
     </row>
@@ -3158,12 +3158,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Cisneros, Melanie</t>
+          <t>Mcclure, Joel</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Melanie.Cisneros@fake_domain.com</t>
+          <t>Joel.Mcclure@fake_domain.com</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -3173,12 +3173,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Green, Sharon</t>
+          <t>Hendricks, Rebecca</t>
         </is>
       </c>
     </row>
@@ -3202,12 +3202,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Robinson, Bruce</t>
+          <t>Short, Angie</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Bruce.Robinson@fake_domain.com</t>
+          <t>Angie.Short@fake_domain.com</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -3217,12 +3217,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Green, Sharon</t>
+          <t>Hendricks, Rebecca</t>
         </is>
       </c>
     </row>
@@ -3246,12 +3246,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Williams, Steven</t>
+          <t>Perez, Kayla</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Steven.Williams@fake_domain.com</t>
+          <t>Kayla.Perez@fake_domain.com</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Green, Sharon</t>
+          <t>Hendricks, Rebecca</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Brewer, Michael</t>
+          <t>Phelps, Zachary</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Michael.Brewer@fake_domain.com</t>
+          <t>Zachary.Phelps@fake_domain.com</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -3305,12 +3305,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Green, Sharon</t>
+          <t>Hendricks, Rebecca</t>
         </is>
       </c>
     </row>
@@ -3334,12 +3334,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Barker, Dawn</t>
+          <t>Spence, Tyler</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Dawn.Barker@fake_domain.com</t>
+          <t>Tyler.Spence@fake_domain.com</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -3349,12 +3349,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Green, Sharon</t>
+          <t>Hendricks, Rebecca</t>
         </is>
       </c>
     </row>
@@ -3378,12 +3378,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Young, Phyllis</t>
+          <t>Henry, Rebecca</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Phyllis.Young@fake_domain.com</t>
+          <t>Rebecca.Henry@fake_domain.com</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -3393,12 +3393,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Carroll, Randy</t>
+          <t>Sanchez, Cameron</t>
         </is>
       </c>
     </row>
@@ -3422,12 +3422,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Shelton, Michael</t>
+          <t>Rodriguez, Alejandro</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Michael.Shelton@fake_domain.com</t>
+          <t>Alejandro.Rodriguez@fake_domain.com</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -3437,12 +3437,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Carroll, Randy</t>
+          <t>Sanchez, Cameron</t>
         </is>
       </c>
     </row>
@@ -3466,12 +3466,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Wiley, Russell</t>
+          <t>Stewart, Gina</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Russell.Wiley@fake_domain.com</t>
+          <t>Gina.Stewart@fake_domain.com</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -3481,12 +3481,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Davis, Angela</t>
+          <t>Meyer, Timothy</t>
         </is>
       </c>
     </row>
@@ -3510,12 +3510,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Osborn, Vicki</t>
+          <t>Alvarez, Betty</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Vicki.Osborn@fake_domain.com</t>
+          <t>Betty.Alvarez@fake_domain.com</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -3525,12 +3525,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Robinson, Philip</t>
+          <t>Irwin, Melissa</t>
         </is>
       </c>
     </row>
@@ -3554,12 +3554,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Adams, Robert</t>
+          <t>Leach, William</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Robert.Adams@fake_domain.com</t>
+          <t>William.Leach@fake_domain.com</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -3569,12 +3569,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Robinson, Philip</t>
+          <t>Irwin, Melissa</t>
         </is>
       </c>
     </row>
@@ -3598,12 +3598,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Casey, Rachel</t>
+          <t>Harris, Marcus</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Rachel.Casey@fake_domain.com</t>
+          <t>Marcus.Harris@fake_domain.com</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -3613,12 +3613,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Robinson, Philip</t>
+          <t>Irwin, Melissa</t>
         </is>
       </c>
     </row>
@@ -3642,12 +3642,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Choi, Edward</t>
+          <t>Miller, Tiffany</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Edward.Choi@fake_domain.com</t>
+          <t>Tiffany.Miller@fake_domain.com</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -3657,12 +3657,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Chandler, Devin</t>
+          <t>Aguilar, Lisa</t>
         </is>
       </c>
     </row>
@@ -3686,12 +3686,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Bailey, Chad</t>
+          <t>Jackson, Jim</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Chad.Bailey@fake_domain.com</t>
+          <t>Jim.Jackson@fake_domain.com</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -3701,12 +3701,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Chandler, Devin</t>
+          <t>Aguilar, Lisa</t>
         </is>
       </c>
     </row>
@@ -3730,12 +3730,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Alexander, Allison</t>
+          <t>Watts, Timothy</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Allison.Alexander@fake_domain.com</t>
+          <t>Timothy.Watts@fake_domain.com</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -3745,12 +3745,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Watkins, Jesse</t>
+          <t>Perez, Nicole</t>
         </is>
       </c>
     </row>
@@ -3774,12 +3774,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Brown, Aaron</t>
+          <t>Hall, Kirk</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Aaron.Brown@fake_domain.com</t>
+          <t>Kirk.Hall@fake_domain.com</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -3789,12 +3789,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Watkins, Jesse</t>
+          <t>Perez, Nicole</t>
         </is>
       </c>
     </row>
@@ -3818,12 +3818,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Howell, Karen</t>
+          <t>Nichols, Phyllis</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Karen.Howell@fake_domain.com</t>
+          <t>Phyllis.Nichols@fake_domain.com</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -3833,12 +3833,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Watkins, Jesse</t>
+          <t>Perez, Nicole</t>
         </is>
       </c>
     </row>
@@ -3862,12 +3862,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Singleton, Jennifer</t>
+          <t>Collins, Jessica</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Jennifer.Singleton@fake_domain.com</t>
+          <t>Jessica.Collins@fake_domain.com</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -3877,12 +3877,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Watkins, Jesse</t>
+          <t>Perez, Nicole</t>
         </is>
       </c>
     </row>
@@ -3906,12 +3906,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Fitzgerald, Natalie</t>
+          <t>Herman, Dawn</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Natalie.Fitzgerald@fake_domain.com</t>
+          <t>Dawn.Herman@fake_domain.com</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -3921,12 +3921,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Watkins, Jesse</t>
+          <t>Perez, Nicole</t>
         </is>
       </c>
     </row>
@@ -3950,12 +3950,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Randall, Sabrina</t>
+          <t>Smith, Nicole</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Sabrina.Randall@fake_domain.com</t>
+          <t>Nicole.Smith@fake_domain.com</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -3965,12 +3965,12 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Blankenship, Mark</t>
+          <t>Warner, John</t>
         </is>
       </c>
     </row>
@@ -3994,12 +3994,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Moore, Ryan</t>
+          <t>Gaines, Shawn</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Ryan.Moore@fake_domain.com</t>
+          <t>Shawn.Gaines@fake_domain.com</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -4009,12 +4009,12 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Blankenship, Mark</t>
+          <t>Warner, John</t>
         </is>
       </c>
     </row>
@@ -4038,12 +4038,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Newman, Sharon</t>
+          <t>Wilson, Katherine</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Sharon.Newman@fake_domain.com</t>
+          <t>Katherine.Wilson@fake_domain.com</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -4053,12 +4053,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Blankenship, Mark</t>
+          <t>Warner, John</t>
         </is>
       </c>
     </row>
@@ -4082,12 +4082,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Mcclain, Jared</t>
+          <t>Gilbert, Gail</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Jared.Mcclain@fake_domain.com</t>
+          <t>Gail.Gilbert@fake_domain.com</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -4097,12 +4097,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Blankenship, Mark</t>
+          <t>Warner, John</t>
         </is>
       </c>
     </row>
@@ -4126,12 +4126,12 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Ortiz, Wayne</t>
+          <t>Parker, Matthew</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Wayne.Ortiz@fake_domain.com</t>
+          <t>Matthew.Parker@fake_domain.com</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -4141,12 +4141,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Blankenship, Mark</t>
+          <t>Warner, John</t>
         </is>
       </c>
     </row>
@@ -4170,12 +4170,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Porter, Louis</t>
+          <t>Wiggins, Noah</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Louis.Porter@fake_domain.com</t>
+          <t>Noah.Wiggins@fake_domain.com</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -4185,12 +4185,12 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Miller, Peter</t>
+          <t>Mercado, Robert</t>
         </is>
       </c>
     </row>
@@ -4214,12 +4214,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Houston, Tyler</t>
+          <t>Romero, Christopher</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Tyler.Houston@fake_domain.com</t>
+          <t>Christopher.Romero@fake_domain.com</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -4229,12 +4229,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Miller, Peter</t>
+          <t>Mercado, Robert</t>
         </is>
       </c>
     </row>
@@ -4258,12 +4258,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Armstrong, Steven</t>
+          <t>Dickerson, Jason</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Steven.Armstrong@fake_domain.com</t>
+          <t>Jason.Dickerson@fake_domain.com</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -4273,12 +4273,12 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Miller, Peter</t>
+          <t>Mercado, Robert</t>
         </is>
       </c>
     </row>
@@ -4370,12 +4370,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Salas, Shannon</t>
+          <t>David Mann, Mr.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Shannon.Salas@fake_domain.com</t>
+          <t>Mr.David.Mann@fake_domain.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -4385,12 +4385,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Mccarthy, Roy</t>
+          <t>Rose, Jacob</t>
         </is>
       </c>
     </row>
@@ -4411,12 +4411,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Mckinney MD, Sara</t>
+          <t>Oliver, Matthew</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Sara.Mckinney.MD@fake_domain.com</t>
+          <t>Matthew.Oliver@fake_domain.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -4426,12 +4426,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Mccarthy, Roy</t>
+          <t>Rose, Jacob</t>
         </is>
       </c>
     </row>
@@ -4452,12 +4452,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mccarthy, Stephanie</t>
+          <t>Schneider, Kayla</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Stephanie.Mccarthy@fake_domain.com</t>
+          <t>Kayla.Schneider@fake_domain.com</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -4467,12 +4467,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Miller, Peter</t>
+          <t>Mercado, Robert</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Perry, Rebecca</t>
+          <t>Walker, Brittany</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Rebecca.Perry@fake_domain.com</t>
+          <t>Brittany.Walker@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Johnson, Paul</t>
+          <t>King, Jill</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Paul.Johnson@fake_domain.com</t>
+          <t>Jill.King@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Knight MD, James</t>
+          <t>Clark, Miranda</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -4592,7 +4592,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>James.Knight.MD@fake_domain.com</t>
+          <t>Miranda.Clark@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sandra.Alvarez@fake_domain.com</t>
+          <t>Andrea.Grant@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4628,7 +4628,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hood, James</t>
+          <t>Porter, Laura</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>James.Hood@fake_domain.com</t>
+          <t>Laura.Porter@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Johnson, Margaret</t>
+          <t>Harvey, Kevin</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Margaret.Johnson@fake_domain.com</t>
+          <t>Kevin.Harvey@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Lambert, Jeremiah</t>
+          <t>Hernandez, Stephanie</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Jeremiah.Lambert@fake_domain.com</t>
+          <t>Stephanie.Hernandez@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Baker, Charles</t>
+          <t>Carter, Lauren</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -4707,7 +4707,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Charles.Baker@fake_domain.com</t>
+          <t>Lauren.Carter@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4720,7 +4720,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Miller, Allison</t>
+          <t>Haas, Matthew</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Allison.Miller@fake_domain.com</t>
+          <t>Matthew.Haas@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Wolfe, Austin</t>
+          <t>Davis, Julie</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -4753,7 +4753,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Austin.Wolfe@fake_domain.com</t>
+          <t>Julie.Davis@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Kane, David</t>
+          <t>Williams, Anna</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -4776,7 +4776,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>David.Kane@fake_domain.com</t>
+          <t>Anna.Williams@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4855,12 +4855,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Johnson, Paul</t>
+          <t>King, Jill</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Paul.Johnson@fake_domain.com</t>
+          <t>Jill.King@fake_domain.com</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -4888,12 +4888,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Perry, Rebecca</t>
+          <t>Walker, Brittany</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Rebecca.Perry@fake_domain.com</t>
+          <t>Brittany.Walker@fake_domain.com</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -4921,12 +4921,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Knight MD, James</t>
+          <t>Clark, Miranda</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>James.Knight.MD@fake_domain.com</t>
+          <t>Miranda.Clark@fake_domain.com</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -4995,22 +4995,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Pamela.Rubio@fake_domain.com</t>
+          <t>Kristen.Wagner@fake_domain.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mccarthy, Roy</t>
+          <t>Rose, Jacob</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Roy.Mccarthy@fake_domain.com</t>
+          <t>Jacob.Rose@fake_domain.com</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -5028,22 +5028,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rubio, Pamela</t>
+          <t>Wagner, Kristen</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pamela.Rubio@fake_domain.com</t>
+          <t>Kristen.Wagner@fake_domain.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Anderson, Zachary</t>
+          <t>Heath, Mary</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Zachary.Anderson@fake_domain.com</t>
+          <t>Mary.Heath@fake_domain.com</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -5061,22 +5061,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Michael.Frank@fake_domain.com</t>
+          <t>Rhonda.Cortez@fake_domain.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Beck, Johnny</t>
+          <t>Ryan, Amy</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Johnny.Beck@fake_domain.com</t>
+          <t>Amy.Ryan@fake_domain.com</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -5094,22 +5094,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Michael.Frank@fake_domain.com</t>
+          <t>Rhonda.Cortez@fake_domain.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Green, Sharon</t>
+          <t>Hendricks, Rebecca</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Sharon.Green@fake_domain.com</t>
+          <t>Rebecca.Hendricks@fake_domain.com</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -5127,22 +5127,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Michael.Frank@fake_domain.com</t>
+          <t>Rhonda.Cortez@fake_domain.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Valdez MD, Kaylee</t>
+          <t>Morgan, William</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Kaylee.Valdez.MD@fake_domain.com</t>
+          <t>William.Morgan@fake_domain.com</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -5160,22 +5160,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Michael.Frank@fake_domain.com</t>
+          <t>Rhonda.Cortez@fake_domain.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Davis, Angela</t>
+          <t>Meyer, Timothy</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Angela.Davis@fake_domain.com</t>
+          <t>Timothy.Meyer@fake_domain.com</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -5193,22 +5193,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Frank, Michael</t>
+          <t>Cortez, Rhonda</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Michael.Frank@fake_domain.com</t>
+          <t>Rhonda.Cortez@fake_domain.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Robinson, Philip</t>
+          <t>Irwin, Melissa</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Philip.Robinson@fake_domain.com</t>
+          <t>Melissa.Irwin@fake_domain.com</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -5226,22 +5226,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sandra.Alvarez@fake_domain.com</t>
+          <t>Andrea.Grant@fake_domain.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Watkins, Jesse</t>
+          <t>Perez, Nicole</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Jesse.Watkins@fake_domain.com</t>
+          <t>Nicole.Perez@fake_domain.com</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -5259,22 +5259,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sandra.Alvarez@fake_domain.com</t>
+          <t>Andrea.Grant@fake_domain.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Blankenship, Mark</t>
+          <t>Warner, John</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Mark.Blankenship@fake_domain.com</t>
+          <t>John.Warner@fake_domain.com</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -5292,22 +5292,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Alvarez, Sandra</t>
+          <t>Grant, Andrea</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Sandra.Alvarez@fake_domain.com</t>
+          <t>Andrea.Grant@fake_domain.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Miller, Peter</t>
+          <t>Mercado, Robert</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Peter.Miller@fake_domain.com</t>
+          <t>Robert.Mercado@fake_domain.com</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -5392,12 +5392,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Torres, Jason</t>
+          <t>Stone, Johnny</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Jason.Torres@fake_domain.com</t>
+          <t>Johnny.Stone@fake_domain.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -5423,12 +5423,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Stewart, Brian</t>
+          <t>Schmitt, Melinda</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Brian.Stewart@fake_domain.com</t>
+          <t>Melinda.Schmitt@fake_domain.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -5454,12 +5454,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Bennett, Susan</t>
+          <t>Anderson, Ronald</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Susan.Bennett@fake_domain.com</t>
+          <t>Ronald.Anderson@fake_domain.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -5485,12 +5485,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Hunt, Whitney</t>
+          <t>Willis, Timothy</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Whitney.Hunt@fake_domain.com</t>
+          <t>Timothy.Willis@fake_domain.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -5516,12 +5516,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Colleen May MD, Mrs.</t>
+          <t>Duke, Jonathan</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Mrs.Colleen.May.MD@fake_domain.com</t>
+          <t>Jonathan.Duke@fake_domain.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -5547,12 +5547,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Perez, Jenny</t>
+          <t>Hamilton, Kelly</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Jenny.Perez@fake_domain.com</t>
+          <t>Kelly.Hamilton@fake_domain.com</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -5578,12 +5578,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Dickerson, Jermaine</t>
+          <t>Linda Gutierrez, Mrs.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Jermaine.Dickerson@fake_domain.com</t>
+          <t>Mrs.Linda.Gutierrez@fake_domain.com</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -5609,12 +5609,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Miller, Emily</t>
+          <t>Schneider, Danielle</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Emily.Miller@fake_domain.com</t>
+          <t>Danielle.Schneider@fake_domain.com</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hinton, Christopher</t>
+          <t>Weeks, Andrew</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -5708,7 +5708,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hinton</t>
+          <t>Weeks</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -5737,7 +5737,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Kline, Michael</t>
+          <t>Pierce, Joel</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -5747,7 +5747,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kline</t>
+          <t>Pierce</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -5776,7 +5776,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Houston, Kathryn</t>
+          <t>Fitzgerald, Michael</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -5786,7 +5786,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Fitzgerald</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -5815,7 +5815,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Dillon, John</t>
+          <t>Johnson, George</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -5825,7 +5825,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dillon</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -5854,7 +5854,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Rogers, Jamie</t>
+          <t>Fisher, Pamela</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -5864,7 +5864,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Rogers</t>
+          <t>Fisher</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -5893,7 +5893,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Rowland, Jennifer</t>
+          <t>Barajas, Robert</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Rowland</t>
+          <t>Barajas</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -5932,7 +5932,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Miller, David</t>
+          <t>Mason, Amy</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -5942,7 +5942,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Mason</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Costa, Holly</t>
+          <t>Ellis, Mikayla</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -5981,7 +5981,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Costa</t>
+          <t>Ellis</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -6010,7 +6010,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Rodgers, Jessica</t>
+          <t>Weaver, Miranda</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -6020,7 +6020,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Rodgers</t>
+          <t>Weaver</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -6049,7 +6049,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Murphy, Matthew</t>
+          <t>Spence, Raymond</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -6059,7 +6059,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Murphy</t>
+          <t>Spence</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Gonzalez, Christopher</t>
+          <t>Brown, Kathleen</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Gonzalez</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -6127,7 +6127,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Brown, Lauren</t>
+          <t>Rogers, Stephen</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Rogers</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -6166,7 +6166,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Miller, Amy</t>
+          <t>Stevens, Tracy</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -6176,7 +6176,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Stevens</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -6205,7 +6205,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Rangel, Christopher</t>
+          <t>Clarke, Carrie</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -6215,7 +6215,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Rangel</t>
+          <t>Clarke</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -6244,7 +6244,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>May, Jordan</t>
+          <t>Acevedo, Sandra</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -6254,7 +6254,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>May</t>
+          <t>Acevedo</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Vargas, Dawn</t>
+          <t>Wolf, Scott</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -6293,7 +6293,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Vargas</t>
+          <t>Wolf</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -6322,7 +6322,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Smith, Jamie</t>
+          <t>Roman, Joshua</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -6332,7 +6332,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Roman</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Kennedy, Peter</t>
+          <t>Griffin, Ann</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -6371,7 +6371,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Kennedy</t>
+          <t>Griffin</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -6400,7 +6400,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>White, Carlos</t>
+          <t>Barnett, Laura</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -6410,7 +6410,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Barnett</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -6439,7 +6439,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Baldwin, Cory</t>
+          <t>Haynes, Cynthia</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Baldwin</t>
+          <t>Haynes</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -6478,7 +6478,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Murphy, Jason</t>
+          <t>Long, Abigail</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -6488,7 +6488,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Murphy</t>
+          <t>Long</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Kidd, Donna</t>
+          <t>Foster, Erica</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -6527,7 +6527,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Kidd</t>
+          <t>Foster</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -6556,7 +6556,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Shannon, Angela</t>
+          <t>Miller, Austin</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -6566,7 +6566,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Shannon</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -6595,7 +6595,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Mendez, Christopher</t>
+          <t>Turner, Maria</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Mendez</t>
+          <t>Turner</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -6634,7 +6634,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Dodson, Ellen</t>
+          <t>Russell, Aaron</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -6644,7 +6644,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Dodson</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -6675,7 +6675,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Nichols, Keith</t>
+          <t>Roberts, Karen</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Nichols</t>
+          <t>Roberts</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -6714,7 +6714,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Perez, Jenny</t>
+          <t>Hamilton, Kelly</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -6724,7 +6724,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Perez</t>
+          <t>Hamilton</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -6753,7 +6753,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tanner, Caroline</t>
+          <t>Williams DVM, Amber</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -6763,7 +6763,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Tanner</t>
+          <t>Williams DVM</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -6792,7 +6792,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Miller, Joseph</t>
+          <t>Bass, David</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -6802,7 +6802,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Bass</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -6831,7 +6831,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Avery, Alyssa</t>
+          <t>Ware, Arthur</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Avery</t>
+          <t>Ware</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -6870,7 +6870,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Hanson, Kim</t>
+          <t>Weiss, Angela</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -6880,7 +6880,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Hanson</t>
+          <t>Weiss</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Griffin, David</t>
+          <t>Simon, Heather</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -6919,7 +6919,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Griffin</t>
+          <t>Simon</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -6948,7 +6948,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Ross, Jennifer</t>
+          <t>Mckenzie, Amanda</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -6958,7 +6958,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Ross</t>
+          <t>Mckenzie</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -6987,7 +6987,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Gutierrez, Timothy</t>
+          <t>Jenkins DVM, Brian</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -6997,7 +6997,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Gutierrez</t>
+          <t>Jenkins DVM</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -7026,7 +7026,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Mosley, Joshua</t>
+          <t>Decker, Kevin</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -7036,7 +7036,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Mosley</t>
+          <t>Decker</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -7065,7 +7065,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Torres, Linda</t>
+          <t>Thomas, Connie</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -7075,7 +7075,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Torres</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -7106,7 +7106,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Bush, Tiffany</t>
+          <t>Weaver, Claudia</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -7116,7 +7116,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Bush</t>
+          <t>Weaver</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -7145,7 +7145,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Hernandez, Alexander</t>
+          <t>Roberts II, Robert</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -7155,7 +7155,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Roberts II</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -7184,7 +7184,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Patterson, Stephanie</t>
+          <t>Hernandez, Matthew</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Patterson</t>
+          <t>Hernandez</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Smith, Zachary</t>
+          <t>Leon, Megan</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -7233,7 +7233,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Leon</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -7262,7 +7262,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Lawson, Kristen</t>
+          <t>Jenkins, Ryan</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -7272,7 +7272,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Lawson</t>
+          <t>Jenkins</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Anderson, Christopher</t>
+          <t>Villarreal, Thomas</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -7311,7 +7311,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Anderson</t>
+          <t>Villarreal</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -7340,7 +7340,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Myers, Kelsey</t>
+          <t>Ryan, Zachary</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -7350,7 +7350,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Myers</t>
+          <t>Ryan</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -7379,7 +7379,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>White, Brenda</t>
+          <t>Davidson, Kelly</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -7389,7 +7389,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Davidson</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -7418,7 +7418,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Harris, David</t>
+          <t>Osborne, Andre</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -7428,7 +7428,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Osborne</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -7457,7 +7457,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Hernandez, William</t>
+          <t>Hopkins, Brianna</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -7467,7 +7467,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Hopkins</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -7496,7 +7496,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Dawson, Jose</t>
+          <t>Garcia, Matthew</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -7506,7 +7506,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Dawson</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -7535,7 +7535,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Leach, Nicholas</t>
+          <t>Wright, Jeremy</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -7545,7 +7545,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Leach</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -7574,7 +7574,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Kelly, Justin</t>
+          <t>Newton, Mark</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Kelly</t>
+          <t>Newton</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -7658,12 +7658,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Carr</t>
+          <t>Peterson</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>Heidi</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -7681,19 +7681,19 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Jennifer.Carr@fake_domain.com</t>
+          <t>Heidi.Peterson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Thompson</t>
+          <t>White</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kyle</t>
+          <t>Diane</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -7711,19 +7711,19 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Kyle.Thompson@fake_domain.com</t>
+          <t>Diane.White@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Caldwell</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -7741,19 +7741,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mary.Stark@fake_domain.com</t>
+          <t>Daniel.Martin@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mclaughlin</t>
+          <t>Ramirez MD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>Vanessa</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -7771,19 +7771,19 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Anthony.Mclaughlin@fake_domain.com</t>
+          <t>Vanessa.Ramirez.MD@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Gonzales</t>
+          <t>Zamora</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Garyan</t>
+          <t>Noahan</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -7801,19 +7801,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Angela.Gonzales@fake_domain.com</t>
+          <t>Scott.Zamora@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Griffith</t>
+          <t>Porter</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kari Glenda.</t>
+          <t>Vanessa Nathan.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -7831,19 +7831,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Kari.Griffith@fake_domain.com</t>
+          <t>Vanessa.Porter@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ward</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jamie </t>
+          <t xml:space="preserve">Jim </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -7861,19 +7861,19 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Jamie.Butler@fake_domain.com</t>
+          <t>Jim.Mitchell@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Grant</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>James I.</t>
+          <t>Teresa I.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -7891,19 +7891,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>James.Grant@fake_domain.com</t>
+          <t>Teresa.Johnson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Phillips</t>
+          <t>Garcia</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>David A.</t>
+          <t>Kayla A.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -7921,19 +7921,19 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>David.Phillips@fake_domain.com</t>
+          <t>Kayla.Garcia@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Valentine</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Derek</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -7951,19 +7951,19 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Daniel.Johnson@fake_domain.com</t>
+          <t>Jamie.Valentine@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Oconnor</t>
+          <t>Hines</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>Ruth</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -7981,19 +7981,19 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Matthew.Oconnor@fake_domain.com</t>
+          <t>Ruth.Hines@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Gordon</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Caitlin</t>
+          <t>Sara</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -8011,19 +8011,19 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Caitlin.Brown@fake_domain.com</t>
+          <t>Sara.Gordon@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mccullough</t>
+          <t>Adams</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DarJason</t>
+          <t>DarVincent</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -8041,19 +8041,19 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Joann.Mccullough@fake_domain.com</t>
+          <t>Paul.Adams@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Cox</t>
+          <t>Gibson</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Brandon</t>
+          <t>Kevin</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -8071,19 +8071,19 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Brandon.Cox@fake_domain.com</t>
+          <t>Kevin.Gibson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Harper</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Chelsear</t>
+          <t>Kathleenr</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -8101,19 +8101,19 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Chelsea.Harper@fake_domain.com</t>
+          <t>Kathleen.Johnson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Hill</t>
+          <t>Pollard</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Garyanette</t>
+          <t>Noahanette</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -8131,19 +8131,19 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Charles.Smith@fake_domain.com</t>
+          <t>Haley.Brewer@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Young</t>
+          <t>Manning</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Wendy</t>
+          <t>Erin</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -8161,19 +8161,19 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Monique.Young@fake_domain.com</t>
+          <t>Joseph.Manning@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Poole</t>
+          <t>Ward</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Daniel Marissa</t>
+          <t>David David</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -8191,19 +8191,19 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel.Poole@fake_domain.com </t>
+          <t xml:space="preserve">David.Ward@fake_domain.com </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Rogers</t>
+          <t>Erickson</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Christopher</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -8221,19 +8221,19 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>John.Rogers@fake_domain.com</t>
+          <t>Christopher.Erickson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Foster</t>
+          <t>Peterson</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>Jeremy</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -8251,19 +8251,19 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Christopher.Foster@fake_domain.com</t>
+          <t>Jeremy.Peterson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Baker</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jackson Glenda.</t>
+          <t>Anna Nathan.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -8281,19 +8281,19 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Jackson.Baker@fake_domain.com</t>
+          <t>Anna.Smith@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Clay</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Kayleelas R.</t>
+          <t>Williamlas R.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -8311,19 +8311,19 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Wayne.Johnston@fake_domain.com</t>
+          <t>Benjamin.Stone@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Clay</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reginald D. </t>
+          <t xml:space="preserve">Sarah D. </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -8341,19 +8341,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Reginald.Barker@fake_domain.com</t>
+          <t>Sarah.May@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Chapman</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Bryan</t>
+          <t>Cody</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -8371,7 +8371,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Bryan.Chapman@fake_domain.com</t>
+          <t>Cody.Jones@fake_domain.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update test inputs with 10-17-22 PEARS schema
</commit_message>
<xml_diff>
--- a/tests/test_inputs/FY23_INEP_Staff_List.xlsx
+++ b/tests/test_inputs/FY23_INEP_Staff_List.xlsx
@@ -2850,12 +2850,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Snyder, Brittany</t>
+          <t>Torres MD, Melinda</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Brittany.Snyder@fake_domain.com</t>
+          <t>Melinda.Torres.MD@fake_domain.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2865,12 +2865,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Rose, Jacob</t>
+          <t>Butler, Lori</t>
         </is>
       </c>
     </row>
@@ -2894,12 +2894,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Velez, Dustin</t>
+          <t>Maldonado, Ernest</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Dustin.Velez@fake_domain.com</t>
+          <t>Ernest.Maldonado@fake_domain.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -2909,12 +2909,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Rose, Jacob</t>
+          <t>Butler, Lori</t>
         </is>
       </c>
     </row>
@@ -2938,12 +2938,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Sparks, Bruce</t>
+          <t>Conway, Jaime</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Bruce.Sparks@fake_domain.com</t>
+          <t>Jaime.Conway@fake_domain.com</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -2953,12 +2953,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Rose, Jacob</t>
+          <t>Butler, Lori</t>
         </is>
       </c>
     </row>
@@ -2982,12 +2982,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Jones, Robert</t>
+          <t>Mcmillan, Elizabeth</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Robert.Jones@fake_domain.com</t>
+          <t>Elizabeth.Mcmillan@fake_domain.com</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -2997,12 +2997,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Rose, Jacob</t>
+          <t>Butler, Lori</t>
         </is>
       </c>
     </row>
@@ -3026,12 +3026,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Martin, Jesse</t>
+          <t>Ramirez, Lindsay</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Jesse.Martin@fake_domain.com</t>
+          <t>Lindsay.Ramirez@fake_domain.com</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -3041,12 +3041,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Rose, Jacob</t>
+          <t>Butler, Lori</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Barnes, Amy</t>
+          <t>Thompson, Rachel</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Amy.Barnes@fake_domain.com</t>
+          <t>Rachel.Thompson@fake_domain.com</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -3085,12 +3085,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Ryan, Amy</t>
+          <t>Hawkins, Matthew</t>
         </is>
       </c>
     </row>
@@ -3114,12 +3114,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Rodgers, David</t>
+          <t>Baldwin, Bobby</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>David.Rodgers@fake_domain.com</t>
+          <t>Bobby.Baldwin@fake_domain.com</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -3129,12 +3129,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Ryan, Amy</t>
+          <t>Hawkins, Matthew</t>
         </is>
       </c>
     </row>
@@ -3158,12 +3158,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Mcclure, Joel</t>
+          <t>Gonzalez, Sarah</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Joel.Mcclure@fake_domain.com</t>
+          <t>Sarah.Gonzalez@fake_domain.com</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -3173,12 +3173,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Hendricks, Rebecca</t>
+          <t>Thompson, Scott</t>
         </is>
       </c>
     </row>
@@ -3202,12 +3202,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Short, Angie</t>
+          <t>Barnes, Daniel</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Angie.Short@fake_domain.com</t>
+          <t>Daniel.Barnes@fake_domain.com</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -3217,12 +3217,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Hendricks, Rebecca</t>
+          <t>Thompson, Scott</t>
         </is>
       </c>
     </row>
@@ -3246,12 +3246,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Perez, Kayla</t>
+          <t>Cook, Walter</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Kayla.Perez@fake_domain.com</t>
+          <t>Walter.Cook@fake_domain.com</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Hendricks, Rebecca</t>
+          <t>Thompson, Scott</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Phelps, Zachary</t>
+          <t>Palmer, Heather</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Zachary.Phelps@fake_domain.com</t>
+          <t>Heather.Palmer@fake_domain.com</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -3305,12 +3305,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Hendricks, Rebecca</t>
+          <t>Thompson, Scott</t>
         </is>
       </c>
     </row>
@@ -3334,12 +3334,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Spence, Tyler</t>
+          <t>Clark, Bryan</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Tyler.Spence@fake_domain.com</t>
+          <t>Bryan.Clark@fake_domain.com</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -3349,12 +3349,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Hendricks, Rebecca</t>
+          <t>Thompson, Scott</t>
         </is>
       </c>
     </row>
@@ -3378,12 +3378,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Henry, Rebecca</t>
+          <t>Munoz, Rhonda</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Rebecca.Henry@fake_domain.com</t>
+          <t>Rhonda.Munoz@fake_domain.com</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -3393,12 +3393,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Sanchez, Cameron</t>
+          <t>Stewart, Jessica</t>
         </is>
       </c>
     </row>
@@ -3422,12 +3422,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Rodriguez, Alejandro</t>
+          <t>Bruce, Jenny</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Alejandro.Rodriguez@fake_domain.com</t>
+          <t>Jenny.Bruce@fake_domain.com</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -3437,12 +3437,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Sanchez, Cameron</t>
+          <t>Stewart, Jessica</t>
         </is>
       </c>
     </row>
@@ -3466,12 +3466,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Stewart, Gina</t>
+          <t>Riley, Jennifer</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Gina.Stewart@fake_domain.com</t>
+          <t>Jennifer.Riley@fake_domain.com</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -3481,12 +3481,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Meyer, Timothy</t>
+          <t>Jacobs, Alexander</t>
         </is>
       </c>
     </row>
@@ -3510,12 +3510,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Alvarez, Betty</t>
+          <t>Wood, Dawn</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Betty.Alvarez@fake_domain.com</t>
+          <t>Dawn.Wood@fake_domain.com</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -3525,12 +3525,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Irwin, Melissa</t>
+          <t>Johnston, Christian</t>
         </is>
       </c>
     </row>
@@ -3554,12 +3554,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Leach, William</t>
+          <t>Nunez, Tracey</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>William.Leach@fake_domain.com</t>
+          <t>Tracey.Nunez@fake_domain.com</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -3569,12 +3569,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Irwin, Melissa</t>
+          <t>Johnston, Christian</t>
         </is>
       </c>
     </row>
@@ -3598,12 +3598,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Harris, Marcus</t>
+          <t>Martin, Jeremiah</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Marcus.Harris@fake_domain.com</t>
+          <t>Jeremiah.Martin@fake_domain.com</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -3613,12 +3613,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Irwin, Melissa</t>
+          <t>Johnston, Christian</t>
         </is>
       </c>
     </row>
@@ -3642,12 +3642,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Miller, Tiffany</t>
+          <t>Lynn, John</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Tiffany.Miller@fake_domain.com</t>
+          <t>John.Lynn@fake_domain.com</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -3657,12 +3657,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Aguilar, Lisa</t>
+          <t>Hamilton, Kimberly</t>
         </is>
       </c>
     </row>
@@ -3686,12 +3686,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Jackson, Jim</t>
+          <t>Terry, Stephanie</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Jim.Jackson@fake_domain.com</t>
+          <t>Stephanie.Terry@fake_domain.com</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -3701,12 +3701,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Aguilar, Lisa</t>
+          <t>Hamilton, Kimberly</t>
         </is>
       </c>
     </row>
@@ -3730,12 +3730,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Watts, Timothy</t>
+          <t>Murphy, Gabrielle</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Timothy.Watts@fake_domain.com</t>
+          <t>Gabrielle.Murphy@fake_domain.com</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -3745,12 +3745,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Perez, Nicole</t>
+          <t>Coffey, Lauren</t>
         </is>
       </c>
     </row>
@@ -3774,12 +3774,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Hall, Kirk</t>
+          <t>Rodriguez, Kevin</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Kirk.Hall@fake_domain.com</t>
+          <t>Kevin.Rodriguez@fake_domain.com</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -3789,12 +3789,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Perez, Nicole</t>
+          <t>Coffey, Lauren</t>
         </is>
       </c>
     </row>
@@ -3818,12 +3818,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Nichols, Phyllis</t>
+          <t>Holmes, William</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Phyllis.Nichols@fake_domain.com</t>
+          <t>William.Holmes@fake_domain.com</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -3833,12 +3833,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Perez, Nicole</t>
+          <t>Coffey, Lauren</t>
         </is>
       </c>
     </row>
@@ -3862,12 +3862,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Collins, Jessica</t>
+          <t>Bell, Gina</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Jessica.Collins@fake_domain.com</t>
+          <t>Gina.Bell@fake_domain.com</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -3877,12 +3877,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Perez, Nicole</t>
+          <t>Coffey, Lauren</t>
         </is>
       </c>
     </row>
@@ -3906,12 +3906,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Herman, Dawn</t>
+          <t>Cervantes PhD, Richard</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Dawn.Herman@fake_domain.com</t>
+          <t>Richard.Cervantes.PhD@fake_domain.com</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -3921,12 +3921,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Perez, Nicole</t>
+          <t>Coffey, Lauren</t>
         </is>
       </c>
     </row>
@@ -3950,12 +3950,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Smith, Nicole</t>
+          <t>Shelton, April</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Nicole.Smith@fake_domain.com</t>
+          <t>April.Shelton@fake_domain.com</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -3965,12 +3965,12 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Warner, John</t>
+          <t>Mendez, Angelica</t>
         </is>
       </c>
     </row>
@@ -3994,12 +3994,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Gaines, Shawn</t>
+          <t>Rodriguez Jr., Jacob</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Shawn.Gaines@fake_domain.com</t>
+          <t>Jacob.Rodriguez.Jr@fake_domain.com</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -4009,12 +4009,12 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Warner, John</t>
+          <t>Mendez, Angelica</t>
         </is>
       </c>
     </row>
@@ -4038,12 +4038,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Wilson, Katherine</t>
+          <t>Goodwin, Mark</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Katherine.Wilson@fake_domain.com</t>
+          <t>Mark.Goodwin@fake_domain.com</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -4053,12 +4053,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Warner, John</t>
+          <t>Mendez, Angelica</t>
         </is>
       </c>
     </row>
@@ -4082,12 +4082,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Gilbert, Gail</t>
+          <t>Briggs, Kristina</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Gail.Gilbert@fake_domain.com</t>
+          <t>Kristina.Briggs@fake_domain.com</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -4097,12 +4097,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Warner, John</t>
+          <t>Mendez, Angelica</t>
         </is>
       </c>
     </row>
@@ -4126,12 +4126,12 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Parker, Matthew</t>
+          <t>Cline, Ann</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Matthew.Parker@fake_domain.com</t>
+          <t>Ann.Cline@fake_domain.com</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -4141,12 +4141,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Warner, John</t>
+          <t>Mendez, Angelica</t>
         </is>
       </c>
     </row>
@@ -4170,12 +4170,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Wiggins, Noah</t>
+          <t>Singh, Tasha</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Noah.Wiggins@fake_domain.com</t>
+          <t>Tasha.Singh@fake_domain.com</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -4185,12 +4185,12 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Mercado, Robert</t>
+          <t>Rodriguez, Victor</t>
         </is>
       </c>
     </row>
@@ -4214,12 +4214,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Romero, Christopher</t>
+          <t>Craig, John</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Christopher.Romero@fake_domain.com</t>
+          <t>John.Craig@fake_domain.com</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -4229,12 +4229,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Mercado, Robert</t>
+          <t>Rodriguez, Victor</t>
         </is>
       </c>
     </row>
@@ -4258,12 +4258,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Dickerson, Jason</t>
+          <t>Jones, Courtney</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Jason.Dickerson@fake_domain.com</t>
+          <t>Courtney.Jones@fake_domain.com</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -4273,12 +4273,12 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Mercado, Robert</t>
+          <t>Rodriguez, Victor</t>
         </is>
       </c>
     </row>
@@ -4370,12 +4370,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>David Mann, Mr.</t>
+          <t>Johnson, Kristen</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Mr.David.Mann@fake_domain.com</t>
+          <t>Kristen.Johnson@fake_domain.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -4385,12 +4385,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Rose, Jacob</t>
+          <t>Butler, Lori</t>
         </is>
       </c>
     </row>
@@ -4411,12 +4411,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Oliver, Matthew</t>
+          <t>West, Carrie</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Matthew.Oliver@fake_domain.com</t>
+          <t>Carrie.West@fake_domain.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -4426,12 +4426,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Rose, Jacob</t>
+          <t>Butler, Lori</t>
         </is>
       </c>
     </row>
@@ -4452,12 +4452,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Schneider, Kayla</t>
+          <t>Vargas, Emily</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Kayla.Schneider@fake_domain.com</t>
+          <t>Emily.Vargas@fake_domain.com</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -4467,12 +4467,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Mercado, Robert</t>
+          <t>Rodriguez, Victor</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Walker, Brittany</t>
+          <t>Camacho, Billy</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Brittany.Walker@fake_domain.com</t>
+          <t>Billy.Camacho@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>King, Jill</t>
+          <t>White, Darren</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Jill.King@fake_domain.com</t>
+          <t>Darren.White@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Clark, Miranda</t>
+          <t>Williams, Kimberly</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -4592,7 +4592,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Miranda.Clark@fake_domain.com</t>
+          <t>Kimberly.Williams@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Andrea.Grant@fake_domain.com</t>
+          <t>Jennifer.Heath@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4628,7 +4628,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Porter, Laura</t>
+          <t>Wagner, Morgan</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Laura.Porter@fake_domain.com</t>
+          <t>Morgan.Wagner@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Harvey, Kevin</t>
+          <t>Baker, Kevin</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Kevin.Harvey@fake_domain.com</t>
+          <t>Kevin.Baker@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Hernandez, Stephanie</t>
+          <t>Jenkins, Timothy</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Stephanie.Hernandez@fake_domain.com</t>
+          <t>Timothy.Jenkins@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Carter, Lauren</t>
+          <t>Garza, Julie</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -4707,7 +4707,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Lauren.Carter@fake_domain.com</t>
+          <t>Julie.Garza@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4720,7 +4720,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Haas, Matthew</t>
+          <t>Levy, Christopher</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Matthew.Haas@fake_domain.com</t>
+          <t>Christopher.Levy@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Davis, Julie</t>
+          <t>Martin, Destiny</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -4753,7 +4753,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Julie.Davis@fake_domain.com</t>
+          <t>Destiny.Martin@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Williams, Anna</t>
+          <t>Ross, Dana</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -4776,7 +4776,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Anna.Williams@fake_domain.com</t>
+          <t>Dana.Ross@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4855,12 +4855,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>King, Jill</t>
+          <t>White, Darren</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Jill.King@fake_domain.com</t>
+          <t>Darren.White@fake_domain.com</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -4888,12 +4888,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Walker, Brittany</t>
+          <t>Camacho, Billy</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Brittany.Walker@fake_domain.com</t>
+          <t>Billy.Camacho@fake_domain.com</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -4921,12 +4921,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Clark, Miranda</t>
+          <t>Williams, Kimberly</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Miranda.Clark@fake_domain.com</t>
+          <t>Kimberly.Williams@fake_domain.com</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -4995,22 +4995,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Kristen.Wagner@fake_domain.com</t>
+          <t>Anne.Chavez@fake_domain.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rose, Jacob</t>
+          <t>Butler, Lori</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Jacob.Rose@fake_domain.com</t>
+          <t>Lori.Butler@fake_domain.com</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -5028,22 +5028,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Wagner, Kristen</t>
+          <t>Chavez, Anne</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Kristen.Wagner@fake_domain.com</t>
+          <t>Anne.Chavez@fake_domain.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Heath, Mary</t>
+          <t>Bridges, John</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Mary.Heath@fake_domain.com</t>
+          <t>John.Bridges@fake_domain.com</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -5061,22 +5061,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Rhonda.Cortez@fake_domain.com</t>
+          <t>Shawn.Russo@fake_domain.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Ryan, Amy</t>
+          <t>Hawkins, Matthew</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Amy.Ryan@fake_domain.com</t>
+          <t>Matthew.Hawkins@fake_domain.com</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -5094,22 +5094,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Rhonda.Cortez@fake_domain.com</t>
+          <t>Shawn.Russo@fake_domain.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hendricks, Rebecca</t>
+          <t>Thompson, Scott</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Rebecca.Hendricks@fake_domain.com</t>
+          <t>Scott.Thompson@fake_domain.com</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -5127,22 +5127,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Rhonda.Cortez@fake_domain.com</t>
+          <t>Shawn.Russo@fake_domain.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Morgan, William</t>
+          <t>Mendez, Adrian</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>William.Morgan@fake_domain.com</t>
+          <t>Adrian.Mendez@fake_domain.com</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -5160,22 +5160,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Rhonda.Cortez@fake_domain.com</t>
+          <t>Shawn.Russo@fake_domain.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Meyer, Timothy</t>
+          <t>Jacobs, Alexander</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Timothy.Meyer@fake_domain.com</t>
+          <t>Alexander.Jacobs@fake_domain.com</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -5193,22 +5193,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cortez, Rhonda</t>
+          <t>Russo, Shawn</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Rhonda.Cortez@fake_domain.com</t>
+          <t>Shawn.Russo@fake_domain.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Irwin, Melissa</t>
+          <t>Johnston, Christian</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Melissa.Irwin@fake_domain.com</t>
+          <t>Christian.Johnston@fake_domain.com</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -5226,22 +5226,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Andrea.Grant@fake_domain.com</t>
+          <t>Jennifer.Heath@fake_domain.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Perez, Nicole</t>
+          <t>Coffey, Lauren</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Nicole.Perez@fake_domain.com</t>
+          <t>Lauren.Coffey@fake_domain.com</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -5259,22 +5259,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Andrea.Grant@fake_domain.com</t>
+          <t>Jennifer.Heath@fake_domain.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Warner, John</t>
+          <t>Mendez, Angelica</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>John.Warner@fake_domain.com</t>
+          <t>Angelica.Mendez@fake_domain.com</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -5292,22 +5292,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Grant, Andrea</t>
+          <t>Heath, Jennifer</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Andrea.Grant@fake_domain.com</t>
+          <t>Jennifer.Heath@fake_domain.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mercado, Robert</t>
+          <t>Rodriguez, Victor</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Robert.Mercado@fake_domain.com</t>
+          <t>Victor.Rodriguez@fake_domain.com</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -5392,12 +5392,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Stone, Johnny</t>
+          <t>Wilkins, Heather</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Johnny.Stone@fake_domain.com</t>
+          <t>Heather.Wilkins@fake_domain.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -5423,12 +5423,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Schmitt, Melinda</t>
+          <t>Garza, Jason</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Melinda.Schmitt@fake_domain.com</t>
+          <t>Jason.Garza@fake_domain.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -5454,12 +5454,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Anderson, Ronald</t>
+          <t>Moore, Megan</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Ronald.Anderson@fake_domain.com</t>
+          <t>Megan.Moore@fake_domain.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -5485,12 +5485,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Willis, Timothy</t>
+          <t>Young, Amanda</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Timothy.Willis@fake_domain.com</t>
+          <t>Amanda.Young@fake_domain.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -5516,12 +5516,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Duke, Jonathan</t>
+          <t>Sanchez, Michael</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Jonathan.Duke@fake_domain.com</t>
+          <t>Michael.Sanchez@fake_domain.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -5547,12 +5547,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Hamilton, Kelly</t>
+          <t>Bass, Joseph</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Kelly.Hamilton@fake_domain.com</t>
+          <t>Joseph.Bass@fake_domain.com</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -5578,12 +5578,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Linda Gutierrez, Mrs.</t>
+          <t>Graham, Denise</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Mrs.Linda.Gutierrez@fake_domain.com</t>
+          <t>Denise.Graham@fake_domain.com</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -5609,12 +5609,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Schneider, Danielle</t>
+          <t>Vega, Autumn</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Danielle.Schneider@fake_domain.com</t>
+          <t>Autumn.Vega@fake_domain.com</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Weeks, Andrew</t>
+          <t>Hartman, Johnathan</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -5708,7 +5708,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Weeks</t>
+          <t>Hartman</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -5737,7 +5737,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Pierce, Joel</t>
+          <t>Miller, Stephanie</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -5747,7 +5747,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pierce</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -5776,7 +5776,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Fitzgerald, Michael</t>
+          <t>Farrell MD, Miguel</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -5786,7 +5786,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Fitzgerald</t>
+          <t>Farrell MD</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -5815,7 +5815,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Johnson, George</t>
+          <t>Flores, Pam</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -5825,7 +5825,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Flores</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -5854,7 +5854,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fisher, Pamela</t>
+          <t>Jennings, Ashley</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -5864,7 +5864,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Fisher</t>
+          <t>Jennings</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -5893,7 +5893,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Barajas, Robert</t>
+          <t>Pacheco, John</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Barajas</t>
+          <t>Pacheco</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -5932,7 +5932,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Mason, Amy</t>
+          <t>Holmes, David</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -5942,7 +5942,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Mason</t>
+          <t>Holmes</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ellis, Mikayla</t>
+          <t>Gilbert, Jennifer</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -5981,7 +5981,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ellis</t>
+          <t>Gilbert</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -6010,7 +6010,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Weaver, Miranda</t>
+          <t>Bond, Jamie</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -6020,7 +6020,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Weaver</t>
+          <t>Bond</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -6049,7 +6049,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Spence, Raymond</t>
+          <t>Walker, Frank</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -6059,7 +6059,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Spence</t>
+          <t>Walker</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Brown, Kathleen</t>
+          <t>Aguirre, Alicia</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Aguirre</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -6127,7 +6127,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Rogers, Stephen</t>
+          <t>Robinson, Nicholas</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Rogers</t>
+          <t>Robinson</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -6166,7 +6166,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Stevens, Tracy</t>
+          <t>Martin, Miranda</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -6176,7 +6176,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Stevens</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -6205,7 +6205,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Clarke, Carrie</t>
+          <t>Bass, Casey</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -6215,7 +6215,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Clarke</t>
+          <t>Bass</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -6244,7 +6244,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Acevedo, Sandra</t>
+          <t>Foster, Lauren</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -6254,7 +6254,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Acevedo</t>
+          <t>Foster</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Wolf, Scott</t>
+          <t>Rodriguez, Kevin</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -6293,7 +6293,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Wolf</t>
+          <t>Rodriguez</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -6322,7 +6322,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Roman, Joshua</t>
+          <t>West, Richard</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -6332,7 +6332,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Roman</t>
+          <t>West</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Griffin, Ann</t>
+          <t>Ramos, Michelle</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -6371,7 +6371,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Griffin</t>
+          <t>Ramos</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -6400,7 +6400,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Barnett, Laura</t>
+          <t>Smith, Elizabeth</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -6410,7 +6410,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Barnett</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -6439,7 +6439,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Haynes, Cynthia</t>
+          <t>Taylor, Daniel</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Haynes</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -6478,7 +6478,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Long, Abigail</t>
+          <t>Colon, Andrew</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -6488,7 +6488,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Long</t>
+          <t>Colon</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Foster, Erica</t>
+          <t>Castillo, Sherri</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -6527,7 +6527,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Foster</t>
+          <t>Castillo</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -6556,7 +6556,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Miller, Austin</t>
+          <t>Burnett, Michele</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -6566,7 +6566,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Burnett</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -6595,7 +6595,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Turner, Maria</t>
+          <t>Atkinson, Crystal</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Turner</t>
+          <t>Atkinson</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -6634,7 +6634,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Russell, Aaron</t>
+          <t>Gomez, Julie</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -6644,7 +6644,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Gomez</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -6675,7 +6675,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Roberts, Karen</t>
+          <t>Smith, Susan</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Roberts</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -6714,7 +6714,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Hamilton, Kelly</t>
+          <t>Bass, Joseph</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -6724,7 +6724,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Hamilton</t>
+          <t>Bass</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -6753,7 +6753,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Williams DVM, Amber</t>
+          <t>Ray, Tracy</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -6763,7 +6763,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Williams DVM</t>
+          <t>Ray</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -6792,7 +6792,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Bass, David</t>
+          <t>Archer, Christine</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -6802,7 +6802,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Archer</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -6831,7 +6831,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Ware, Arthur</t>
+          <t>Brown, Connor</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Ware</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -6870,7 +6870,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Weiss, Angela</t>
+          <t>Keller, Sarah</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -6880,7 +6880,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Weiss</t>
+          <t>Keller</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Simon, Heather</t>
+          <t>Soto, Thomas</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -6919,7 +6919,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Soto</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -6948,7 +6948,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Mckenzie, Amanda</t>
+          <t>Thompson, Paige</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -6958,7 +6958,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Mckenzie</t>
+          <t>Thompson</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -6987,7 +6987,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Jenkins DVM, Brian</t>
+          <t>Walls, Douglas</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -6997,7 +6997,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Jenkins DVM</t>
+          <t>Walls</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -7026,7 +7026,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Decker, Kevin</t>
+          <t>Burke, Henry</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -7036,7 +7036,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Decker</t>
+          <t>Burke</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -7065,7 +7065,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Thomas, Connie</t>
+          <t>Burnett, Howard</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -7075,7 +7075,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Burnett</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -7106,7 +7106,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Weaver, Claudia</t>
+          <t>Kenneth Stephens, Mr.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -7116,7 +7116,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Weaver</t>
+          <t>Kenneth Stephens</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -7145,7 +7145,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Roberts II, Robert</t>
+          <t>Jackson, Elizabeth</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -7155,7 +7155,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Roberts II</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -7184,7 +7184,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Hernandez, Matthew</t>
+          <t>Mosley, Alexis</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Mosley</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Leon, Megan</t>
+          <t>Doyle PhD, Margaret</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -7233,7 +7233,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Leon</t>
+          <t>Doyle PhD</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -7262,7 +7262,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Jenkins, Ryan</t>
+          <t>Combs, Eric</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -7272,7 +7272,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Jenkins</t>
+          <t>Combs</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Villarreal, Thomas</t>
+          <t>Booth, Richard</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -7311,7 +7311,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Villarreal</t>
+          <t>Booth</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -7340,7 +7340,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Ryan, Zachary</t>
+          <t>Walton, Loretta</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -7350,7 +7350,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Ryan</t>
+          <t>Walton</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -7379,7 +7379,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Davidson, Kelly</t>
+          <t>Owens, Brian</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -7389,7 +7389,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Davidson</t>
+          <t>Owens</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -7418,7 +7418,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Osborne, Andre</t>
+          <t>Munoz, Joshua</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -7428,7 +7428,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Osborne</t>
+          <t>Munoz</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -7457,7 +7457,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Hopkins, Brianna</t>
+          <t>Green, Danielle</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -7467,7 +7467,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Hopkins</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -7496,7 +7496,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Garcia, Matthew</t>
+          <t>Velasquez, Jeffrey</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -7506,7 +7506,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Velasquez</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -7535,7 +7535,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Wright, Jeremy</t>
+          <t>Bowman, Katherine</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -7545,7 +7545,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Wright</t>
+          <t>Bowman</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -7574,7 +7574,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Newton, Mark</t>
+          <t>Thomas, Mary</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Newton</t>
+          <t>Thomas</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -7658,12 +7658,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Peterson</t>
+          <t>Sampson</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Heidi</t>
+          <t>Brian</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -7681,19 +7681,19 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Heidi.Peterson@fake_domain.com</t>
+          <t>Brian.Sampson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Molina</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Diane</t>
+          <t>Bradley</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -7711,19 +7711,19 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Diane.White@fake_domain.com</t>
+          <t>Bradley.Molina@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Caldwell</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -7741,19 +7741,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Daniel.Martin@fake_domain.com</t>
+          <t>Michael.Norton@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ramirez MD</t>
+          <t>Joseph</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vanessa</t>
+          <t>Leah</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -7771,19 +7771,19 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Vanessa.Ramirez.MD@fake_domain.com</t>
+          <t>Leah.Joseph@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Zamora</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Noahan</t>
+          <t>Amberan</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -7801,19 +7801,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Scott.Zamora@fake_domain.com</t>
+          <t>Lawrence.Marshall@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Porter</t>
+          <t>Hughes</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Vanessa Nathan.</t>
+          <t>Carrie Nathan.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -7831,19 +7831,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Vanessa.Porter@fake_domain.com</t>
+          <t>Carrie.Hughes@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Brooks</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jim </t>
+          <t xml:space="preserve">Jason </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -7861,19 +7861,19 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Jim.Mitchell@fake_domain.com</t>
+          <t>Jason.David@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Wilcox</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Teresa I.</t>
+          <t>Melissa I.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -7891,19 +7891,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Teresa.Johnson@fake_domain.com</t>
+          <t>Melissa.Wilcox@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Griffin</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kayla A.</t>
+          <t>Linda A.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -7921,19 +7921,19 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Kayla.Garcia@fake_domain.com</t>
+          <t>Linda.Griffin@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Valentine</t>
+          <t>Miller</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Melissa</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -7951,19 +7951,19 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Jamie.Valentine@fake_domain.com</t>
+          <t>Stephanie.Miller@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hines</t>
+          <t>Oliver</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ruth</t>
+          <t>Russell</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -7981,19 +7981,19 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Ruth.Hines@fake_domain.com</t>
+          <t>Russell.Oliver@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Gordon</t>
+          <t>Allen</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sara</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -8011,19 +8011,19 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Sara.Gordon@fake_domain.com</t>
+          <t>Craig.Allen@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Adams</t>
+          <t>Schroeder</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DarVincent</t>
+          <t>DarAlex</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -8041,19 +8041,19 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Paul.Adams@fake_domain.com</t>
+          <t>Elizabeth.Schroeder@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Gibson</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Kevin</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -8071,19 +8071,19 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Kevin.Gibson@fake_domain.com</t>
+          <t>Michael.Wilson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Burnett</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kathleenr</t>
+          <t>Calvinr</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -8101,19 +8101,19 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Kathleen.Johnson@fake_domain.com</t>
+          <t>Calvin.Burnett@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Pollard</t>
+          <t>Richardson</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Noahanette</t>
+          <t>Amberanette</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -8131,19 +8131,19 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Haley.Brewer@fake_domain.com</t>
+          <t>Christopher.White@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Manning</t>
+          <t>Burgess DVM</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Erin</t>
+          <t>Julia</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -8161,19 +8161,19 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Joseph.Manning@fake_domain.com</t>
+          <t>Danielle.Burgess.DVM@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Ward</t>
+          <t>Lopez</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>David David</t>
+          <t>Joshua Cheryl</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -8191,19 +8191,19 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">David.Ward@fake_domain.com </t>
+          <t xml:space="preserve">Joshua.Lopez@fake_domain.com </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Erickson</t>
+          <t>Barker</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -8221,19 +8221,19 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Christopher.Erickson@fake_domain.com</t>
+          <t>Ashley.Barker@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Peterson</t>
+          <t>Cooper</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jeremy</t>
+          <t>Deborah</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -8251,19 +8251,19 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Jeremy.Peterson@fake_domain.com</t>
+          <t>Deborah.Cooper@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Alvarado</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Anna Nathan.</t>
+          <t>Rebecca Nathan.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -8281,19 +8281,19 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Anna.Smith@fake_domain.com</t>
+          <t>Rebecca.Alvarado@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Williamlas R.</t>
+          <t>Adrianlas R.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -8311,19 +8311,19 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Benjamin.Stone@fake_domain.com</t>
+          <t>Michael.Lopez@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sarah D. </t>
+          <t xml:space="preserve">James D. </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -8341,19 +8341,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Sarah.May@fake_domain.com</t>
+          <t>James.Shannon@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Natasha Alexander MD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cody</t>
+          <t>Dr.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -8371,7 +8371,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Cody.Jones@fake_domain.com</t>
+          <t>Dr.Natasha.Alexander.MD@fake_domain.com</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update input files to pass test_sheet_fields() in test_pears.py
</commit_message>
<xml_diff>
--- a/tests/test_inputs/FY23_INEP_Staff_List.xlsx
+++ b/tests/test_inputs/FY23_INEP_Staff_List.xlsx
@@ -2850,12 +2850,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Torres MD, Melinda</t>
+          <t>Gibson, Richard</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Melinda.Torres.MD@fake_domain.com</t>
+          <t>Richard.Gibson@fake_domain.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2865,12 +2865,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Butler, Lori</t>
+          <t>Clark, Alicia</t>
         </is>
       </c>
     </row>
@@ -2894,12 +2894,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Maldonado, Ernest</t>
+          <t>Stone, Anthony</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Ernest.Maldonado@fake_domain.com</t>
+          <t>Anthony.Stone@fake_domain.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -2909,12 +2909,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Butler, Lori</t>
+          <t>Clark, Alicia</t>
         </is>
       </c>
     </row>
@@ -2938,12 +2938,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Conway, Jaime</t>
+          <t>Gilbert, Anne</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Jaime.Conway@fake_domain.com</t>
+          <t>Anne.Gilbert@fake_domain.com</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -2953,12 +2953,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Butler, Lori</t>
+          <t>Clark, Alicia</t>
         </is>
       </c>
     </row>
@@ -2982,12 +2982,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Mcmillan, Elizabeth</t>
+          <t>Guerrero, Kimberly</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Elizabeth.Mcmillan@fake_domain.com</t>
+          <t>Kimberly.Guerrero@fake_domain.com</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -2997,12 +2997,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Butler, Lori</t>
+          <t>Clark, Alicia</t>
         </is>
       </c>
     </row>
@@ -3026,12 +3026,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Ramirez, Lindsay</t>
+          <t>Garcia, Kayla</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Lindsay.Ramirez@fake_domain.com</t>
+          <t>Kayla.Garcia@fake_domain.com</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -3041,12 +3041,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Butler, Lori</t>
+          <t>Clark, Alicia</t>
         </is>
       </c>
     </row>
@@ -3070,12 +3070,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Thompson, Rachel</t>
+          <t>Rojas, Richard</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Rachel.Thompson@fake_domain.com</t>
+          <t>Richard.Rojas@fake_domain.com</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -3085,12 +3085,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Hawkins, Matthew</t>
+          <t>Smith, Mark</t>
         </is>
       </c>
     </row>
@@ -3114,12 +3114,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Baldwin, Bobby</t>
+          <t>Yang, Michael</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Bobby.Baldwin@fake_domain.com</t>
+          <t>Michael.Yang@fake_domain.com</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -3129,12 +3129,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Hawkins, Matthew</t>
+          <t>Smith, Mark</t>
         </is>
       </c>
     </row>
@@ -3158,12 +3158,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Gonzalez, Sarah</t>
+          <t>Montgomery, Dalton</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Sarah.Gonzalez@fake_domain.com</t>
+          <t>Dalton.Montgomery@fake_domain.com</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -3173,12 +3173,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Thompson, Scott</t>
+          <t>Smith, Daniel</t>
         </is>
       </c>
     </row>
@@ -3202,12 +3202,12 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Barnes, Daniel</t>
+          <t>Knox, Jason</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Daniel.Barnes@fake_domain.com</t>
+          <t>Jason.Knox@fake_domain.com</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -3217,12 +3217,12 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Thompson, Scott</t>
+          <t>Smith, Daniel</t>
         </is>
       </c>
     </row>
@@ -3246,12 +3246,12 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Cook, Walter</t>
+          <t>Sellers, Jason</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Walter.Cook@fake_domain.com</t>
+          <t>Jason.Sellers@fake_domain.com</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Thompson, Scott</t>
+          <t>Smith, Daniel</t>
         </is>
       </c>
     </row>
@@ -3290,12 +3290,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Palmer, Heather</t>
+          <t>King, Molly</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Heather.Palmer@fake_domain.com</t>
+          <t>Molly.King@fake_domain.com</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -3305,12 +3305,12 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Thompson, Scott</t>
+          <t>Smith, Daniel</t>
         </is>
       </c>
     </row>
@@ -3334,12 +3334,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Clark, Bryan</t>
+          <t>Williams, Richard</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Bryan.Clark@fake_domain.com</t>
+          <t>Richard.Williams@fake_domain.com</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -3349,12 +3349,12 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Thompson, Scott</t>
+          <t>Smith, Daniel</t>
         </is>
       </c>
     </row>
@@ -3378,12 +3378,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Munoz, Rhonda</t>
+          <t>Bell, Adam</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Rhonda.Munoz@fake_domain.com</t>
+          <t>Adam.Bell@fake_domain.com</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -3393,12 +3393,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Stewart, Jessica</t>
+          <t>Martin, John</t>
         </is>
       </c>
     </row>
@@ -3422,12 +3422,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Bruce, Jenny</t>
+          <t>White, Courtney</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Jenny.Bruce@fake_domain.com</t>
+          <t>Courtney.White@fake_domain.com</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -3437,12 +3437,12 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Stewart, Jessica</t>
+          <t>Martin, John</t>
         </is>
       </c>
     </row>
@@ -3466,12 +3466,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Riley, Jennifer</t>
+          <t>Morrison, Caroline</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Jennifer.Riley@fake_domain.com</t>
+          <t>Caroline.Morrison@fake_domain.com</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -3481,12 +3481,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Jacobs, Alexander</t>
+          <t>Gomez, Margaret</t>
         </is>
       </c>
     </row>
@@ -3510,12 +3510,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Wood, Dawn</t>
+          <t>Miller, Rhonda</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Dawn.Wood@fake_domain.com</t>
+          <t>Rhonda.Miller@fake_domain.com</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -3525,12 +3525,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Johnston, Christian</t>
+          <t>Elliott, Sara</t>
         </is>
       </c>
     </row>
@@ -3554,12 +3554,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Nunez, Tracey</t>
+          <t>Williams, Allison</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Tracey.Nunez@fake_domain.com</t>
+          <t>Allison.Williams@fake_domain.com</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -3569,12 +3569,12 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Johnston, Christian</t>
+          <t>Elliott, Sara</t>
         </is>
       </c>
     </row>
@@ -3598,12 +3598,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Martin, Jeremiah</t>
+          <t>Schwartz MD, Lisa</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Jeremiah.Martin@fake_domain.com</t>
+          <t>Lisa.Schwartz.MD@fake_domain.com</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -3613,12 +3613,12 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Johnston, Christian</t>
+          <t>Elliott, Sara</t>
         </is>
       </c>
     </row>
@@ -3642,12 +3642,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Lynn, John</t>
+          <t>Wheeler, Joseph</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>John.Lynn@fake_domain.com</t>
+          <t>Joseph.Wheeler@fake_domain.com</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -3657,12 +3657,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Hamilton, Kimberly</t>
+          <t>Powers, Timothy</t>
         </is>
       </c>
     </row>
@@ -3686,12 +3686,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Terry, Stephanie</t>
+          <t>Thomas, Sandra</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Stephanie.Terry@fake_domain.com</t>
+          <t>Sandra.Thomas@fake_domain.com</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -3701,12 +3701,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Hamilton, Kimberly</t>
+          <t>Powers, Timothy</t>
         </is>
       </c>
     </row>
@@ -3730,12 +3730,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Murphy, Gabrielle</t>
+          <t>Howard, Matthew</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Gabrielle.Murphy@fake_domain.com</t>
+          <t>Matthew.Howard@fake_domain.com</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -3745,12 +3745,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Coffey, Lauren</t>
+          <t>Davis, Angela</t>
         </is>
       </c>
     </row>
@@ -3774,12 +3774,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Rodriguez, Kevin</t>
+          <t>Price, Michelle</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Kevin.Rodriguez@fake_domain.com</t>
+          <t>Michelle.Price@fake_domain.com</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -3789,12 +3789,12 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Coffey, Lauren</t>
+          <t>Davis, Angela</t>
         </is>
       </c>
     </row>
@@ -3818,12 +3818,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Holmes, William</t>
+          <t>Hill, Hannah</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>William.Holmes@fake_domain.com</t>
+          <t>Hannah.Hill@fake_domain.com</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -3833,12 +3833,12 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Coffey, Lauren</t>
+          <t>Davis, Angela</t>
         </is>
       </c>
     </row>
@@ -3862,12 +3862,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Bell, Gina</t>
+          <t>Yang, Brenda</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Gina.Bell@fake_domain.com</t>
+          <t>Brenda.Yang@fake_domain.com</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -3877,12 +3877,12 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Coffey, Lauren</t>
+          <t>Davis, Angela</t>
         </is>
       </c>
     </row>
@@ -3906,12 +3906,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Cervantes PhD, Richard</t>
+          <t>Caldwell, Elizabeth</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Richard.Cervantes.PhD@fake_domain.com</t>
+          <t>Elizabeth.Caldwell@fake_domain.com</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -3921,12 +3921,12 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Coffey, Lauren</t>
+          <t>Davis, Angela</t>
         </is>
       </c>
     </row>
@@ -3950,12 +3950,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Shelton, April</t>
+          <t>Hernandez, Henry</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>April.Shelton@fake_domain.com</t>
+          <t>Henry.Hernandez@fake_domain.com</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -3965,12 +3965,12 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Mendez, Angelica</t>
+          <t>Gray, Stuart</t>
         </is>
       </c>
     </row>
@@ -3994,12 +3994,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Rodriguez Jr., Jacob</t>
+          <t>Rodriguez, Stephanie</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Jacob.Rodriguez.Jr@fake_domain.com</t>
+          <t>Stephanie.Rodriguez@fake_domain.com</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -4009,12 +4009,12 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Mendez, Angelica</t>
+          <t>Gray, Stuart</t>
         </is>
       </c>
     </row>
@@ -4038,12 +4038,12 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Goodwin, Mark</t>
+          <t>Davis, Matthew</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Mark.Goodwin@fake_domain.com</t>
+          <t>Matthew.Davis@fake_domain.com</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -4053,12 +4053,12 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Mendez, Angelica</t>
+          <t>Gray, Stuart</t>
         </is>
       </c>
     </row>
@@ -4082,12 +4082,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Briggs, Kristina</t>
+          <t>Murray, Rachel</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Kristina.Briggs@fake_domain.com</t>
+          <t>Rachel.Murray@fake_domain.com</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -4097,12 +4097,12 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Mendez, Angelica</t>
+          <t>Gray, Stuart</t>
         </is>
       </c>
     </row>
@@ -4126,12 +4126,12 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Cline, Ann</t>
+          <t>Copeland, Sheila</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Ann.Cline@fake_domain.com</t>
+          <t>Sheila.Copeland@fake_domain.com</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -4141,12 +4141,12 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Mendez, Angelica</t>
+          <t>Gray, Stuart</t>
         </is>
       </c>
     </row>
@@ -4170,12 +4170,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Singh, Tasha</t>
+          <t>Gallagher, Elizabeth</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Tasha.Singh@fake_domain.com</t>
+          <t>Elizabeth.Gallagher@fake_domain.com</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -4185,12 +4185,12 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Rodriguez, Victor</t>
+          <t>King, Tracey</t>
         </is>
       </c>
     </row>
@@ -4214,12 +4214,12 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Craig, John</t>
+          <t>Welch, Tiffany</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>John.Craig@fake_domain.com</t>
+          <t>Tiffany.Welch@fake_domain.com</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -4229,12 +4229,12 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Rodriguez, Victor</t>
+          <t>King, Tracey</t>
         </is>
       </c>
     </row>
@@ -4258,12 +4258,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Jones, Courtney</t>
+          <t>Cantrell, Jennifer</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Courtney.Jones@fake_domain.com</t>
+          <t>Jennifer.Cantrell@fake_domain.com</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -4273,12 +4273,12 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Rodriguez, Victor</t>
+          <t>King, Tracey</t>
         </is>
       </c>
     </row>
@@ -4370,12 +4370,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Johnson, Kristen</t>
+          <t>Newton, Sarah</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Kristen.Johnson@fake_domain.com</t>
+          <t>Sarah.Newton@fake_domain.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -4385,12 +4385,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Butler, Lori</t>
+          <t>Clark, Alicia</t>
         </is>
       </c>
     </row>
@@ -4411,12 +4411,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>West, Carrie</t>
+          <t>Berry, Michelle</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Carrie.West@fake_domain.com</t>
+          <t>Michelle.Berry@fake_domain.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -4426,12 +4426,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Butler, Lori</t>
+          <t>Clark, Alicia</t>
         </is>
       </c>
     </row>
@@ -4452,12 +4452,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Vargas, Emily</t>
+          <t>Olson, David</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Emily.Vargas@fake_domain.com</t>
+          <t>David.Olson@fake_domain.com</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -4467,12 +4467,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Rodriguez, Victor</t>
+          <t>King, Tracey</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Camacho, Billy</t>
+          <t>Vincent, Debra</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Billy.Camacho@fake_domain.com</t>
+          <t>Debra.Vincent@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>White, Darren</t>
+          <t>Ryan, Nicole</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Darren.White@fake_domain.com</t>
+          <t>Nicole.Ryan@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Williams, Kimberly</t>
+          <t>Pitts, Stephanie</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -4592,7 +4592,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Kimberly.Williams@fake_domain.com</t>
+          <t>Stephanie.Pitts@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Jennifer.Heath@fake_domain.com</t>
+          <t>Kim.Martinez@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4628,7 +4628,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Wagner, Morgan</t>
+          <t>Smith, James</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -4638,7 +4638,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Morgan.Wagner@fake_domain.com</t>
+          <t>James.Smith@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Baker, Kevin</t>
+          <t>Ibarra, Brian</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Kevin.Baker@fake_domain.com</t>
+          <t>Brian.Ibarra@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Jenkins, Timothy</t>
+          <t>West, Kelly</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Timothy.Jenkins@fake_domain.com</t>
+          <t>Kelly.West@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Garza, Julie</t>
+          <t>Campbell, Ronald</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -4707,7 +4707,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Julie.Garza@fake_domain.com</t>
+          <t>Ronald.Campbell@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4720,7 +4720,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Levy, Christopher</t>
+          <t>Alexander, Benjamin</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Christopher.Levy@fake_domain.com</t>
+          <t>Benjamin.Alexander@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Martin, Destiny</t>
+          <t>Stanton, Charles</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -4753,7 +4753,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Destiny.Martin@fake_domain.com</t>
+          <t>Charles.Stanton@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ross, Dana</t>
+          <t>Schultz, Alexandra</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -4776,7 +4776,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Dana.Ross@fake_domain.com</t>
+          <t>Alexandra.Schultz@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -4855,12 +4855,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>White, Darren</t>
+          <t>Ryan, Nicole</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Darren.White@fake_domain.com</t>
+          <t>Nicole.Ryan@fake_domain.com</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -4888,12 +4888,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Camacho, Billy</t>
+          <t>Vincent, Debra</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Billy.Camacho@fake_domain.com</t>
+          <t>Debra.Vincent@fake_domain.com</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -4921,12 +4921,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Williams, Kimberly</t>
+          <t>Pitts, Stephanie</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Kimberly.Williams@fake_domain.com</t>
+          <t>Stephanie.Pitts@fake_domain.com</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -4995,22 +4995,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Anne.Chavez@fake_domain.com</t>
+          <t>Kimberly.Sanchez@fake_domain.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Butler, Lori</t>
+          <t>Clark, Alicia</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Lori.Butler@fake_domain.com</t>
+          <t>Alicia.Clark@fake_domain.com</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -5028,22 +5028,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Chavez, Anne</t>
+          <t>Sanchez, Kimberly</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Anne.Chavez@fake_domain.com</t>
+          <t>Kimberly.Sanchez@fake_domain.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bridges, John</t>
+          <t>Hanson, Mary</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>John.Bridges@fake_domain.com</t>
+          <t>Mary.Hanson@fake_domain.com</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -5061,22 +5061,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Shawn.Russo@fake_domain.com</t>
+          <t>Kevin.Brown@fake_domain.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Hawkins, Matthew</t>
+          <t>Smith, Mark</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Matthew.Hawkins@fake_domain.com</t>
+          <t>Mark.Smith@fake_domain.com</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -5094,22 +5094,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Shawn.Russo@fake_domain.com</t>
+          <t>Kevin.Brown@fake_domain.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Thompson, Scott</t>
+          <t>Smith, Daniel</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Scott.Thompson@fake_domain.com</t>
+          <t>Daniel.Smith@fake_domain.com</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -5127,22 +5127,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Shawn.Russo@fake_domain.com</t>
+          <t>Kevin.Brown@fake_domain.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Mendez, Adrian</t>
+          <t>Roberts, Miguel</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Adrian.Mendez@fake_domain.com</t>
+          <t>Miguel.Roberts@fake_domain.com</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -5160,22 +5160,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Shawn.Russo@fake_domain.com</t>
+          <t>Kevin.Brown@fake_domain.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Jacobs, Alexander</t>
+          <t>Gomez, Margaret</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Alexander.Jacobs@fake_domain.com</t>
+          <t>Margaret.Gomez@fake_domain.com</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -5193,22 +5193,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Russo, Shawn</t>
+          <t>Brown, Kevin</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Shawn.Russo@fake_domain.com</t>
+          <t>Kevin.Brown@fake_domain.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Johnston, Christian</t>
+          <t>Elliott, Sara</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Christian.Johnston@fake_domain.com</t>
+          <t>Sara.Elliott@fake_domain.com</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -5226,22 +5226,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Jennifer.Heath@fake_domain.com</t>
+          <t>Kim.Martinez@fake_domain.com</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Coffey, Lauren</t>
+          <t>Davis, Angela</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Lauren.Coffey@fake_domain.com</t>
+          <t>Angela.Davis@fake_domain.com</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -5259,22 +5259,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Jennifer.Heath@fake_domain.com</t>
+          <t>Kim.Martinez@fake_domain.com</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Mendez, Angelica</t>
+          <t>Gray, Stuart</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Angelica.Mendez@fake_domain.com</t>
+          <t>Stuart.Gray@fake_domain.com</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -5292,22 +5292,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Heath, Jennifer</t>
+          <t>Martinez, Kim</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Jennifer.Heath@fake_domain.com</t>
+          <t>Kim.Martinez@fake_domain.com</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Rodriguez, Victor</t>
+          <t>King, Tracey</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Victor.Rodriguez@fake_domain.com</t>
+          <t>Tracey.King@fake_domain.com</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -5392,12 +5392,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Wilkins, Heather</t>
+          <t>Howe, Jennifer</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Heather.Wilkins@fake_domain.com</t>
+          <t>Jennifer.Howe@fake_domain.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -5423,12 +5423,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Garza, Jason</t>
+          <t>Jones, Christina</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Jason.Garza@fake_domain.com</t>
+          <t>Christina.Jones@fake_domain.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -5454,12 +5454,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Moore, Megan</t>
+          <t>Beck, Melissa</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Megan.Moore@fake_domain.com</t>
+          <t>Melissa.Beck@fake_domain.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -5485,12 +5485,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Young, Amanda</t>
+          <t>Natalie Benitez, Dr.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Amanda.Young@fake_domain.com</t>
+          <t>Dr.Natalie.Benitez@fake_domain.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -5516,12 +5516,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Sanchez, Michael</t>
+          <t>Walker, Kimberly</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Michael.Sanchez@fake_domain.com</t>
+          <t>Kimberly.Walker@fake_domain.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -5547,12 +5547,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Bass, Joseph</t>
+          <t>Reyes, Adrian</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Joseph.Bass@fake_domain.com</t>
+          <t>Adrian.Reyes@fake_domain.com</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -5578,12 +5578,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Graham, Denise</t>
+          <t>John Silva, Mr.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Denise.Graham@fake_domain.com</t>
+          <t>Mr.John.Silva@fake_domain.com</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -5609,12 +5609,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Vega, Autumn</t>
+          <t>Coleman, Grant</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Autumn.Vega@fake_domain.com</t>
+          <t>Grant.Coleman@fake_domain.com</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hartman, Johnathan</t>
+          <t>Boyd PhD, Craig</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -5708,7 +5708,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hartman</t>
+          <t>Boyd PhD</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -5737,7 +5737,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Miller, Stephanie</t>
+          <t>Lewis, Melissa</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -5747,7 +5747,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Lewis</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -5776,7 +5776,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Farrell MD, Miguel</t>
+          <t>Moore, Allison</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -5786,7 +5786,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Farrell MD</t>
+          <t>Moore</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -5815,7 +5815,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Flores, Pam</t>
+          <t>Armstrong, Daniel</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -5825,7 +5825,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>Armstrong</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -5854,7 +5854,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jennings, Ashley</t>
+          <t>Sanders, Russell</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -5864,7 +5864,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Jennings</t>
+          <t>Sanders</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -5893,7 +5893,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Pacheco, John</t>
+          <t>Rivers, Brandon</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Pacheco</t>
+          <t>Rivers</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -5932,7 +5932,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Holmes, David</t>
+          <t>Tucker, Devin</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -5942,7 +5942,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Holmes</t>
+          <t>Tucker</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Gilbert, Jennifer</t>
+          <t>Gonzalez, Rhonda</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -5981,7 +5981,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Gilbert</t>
+          <t>Gonzalez</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -6010,7 +6010,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bond, Jamie</t>
+          <t>Price, Nicole</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -6020,7 +6020,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Bond</t>
+          <t>Price</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -6049,7 +6049,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Walker, Frank</t>
+          <t>Lee, Mckenzie</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -6059,7 +6059,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Walker</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -6088,7 +6088,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Aguirre, Alicia</t>
+          <t>Fitzgerald, Lisa</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Aguirre</t>
+          <t>Fitzgerald</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -6127,7 +6127,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Robinson, Nicholas</t>
+          <t>Johnson, Amanda</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Robinson</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -6166,7 +6166,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Martin, Miranda</t>
+          <t>Ashley, Ryan</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -6176,7 +6176,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Ashley</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -6205,7 +6205,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Bass, Casey</t>
+          <t>Hill, Abigail</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -6215,7 +6215,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Hill</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -6244,7 +6244,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Foster, Lauren</t>
+          <t>Wells, Deborah</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -6254,7 +6254,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Foster</t>
+          <t>Wells</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Rodriguez, Kevin</t>
+          <t>Elliott, Donna</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -6293,7 +6293,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Rodriguez</t>
+          <t>Elliott</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -6322,7 +6322,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>West, Richard</t>
+          <t>Spears, Stephen</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -6332,7 +6332,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>West</t>
+          <t>Spears</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ramos, Michelle</t>
+          <t>Robertson, Melissa</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -6371,7 +6371,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Ramos</t>
+          <t>Robertson</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -6400,7 +6400,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Smith, Elizabeth</t>
+          <t>Michelle Brown, Mrs.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -6410,7 +6410,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Michelle Brown</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -6439,7 +6439,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Taylor, Daniel</t>
+          <t>Mcintyre, Lisa</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Taylor</t>
+          <t>Mcintyre</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -6478,7 +6478,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Colon, Andrew</t>
+          <t>Smith, Justin</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -6488,7 +6488,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Colon</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Castillo, Sherri</t>
+          <t>Scott, Herbert</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -6527,7 +6527,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Castillo</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -6556,7 +6556,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Burnett, Michele</t>
+          <t>Wilson, Arthur</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -6566,7 +6566,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Burnett</t>
+          <t>Wilson</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -6595,7 +6595,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Atkinson, Crystal</t>
+          <t>Pena, Carla</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Atkinson</t>
+          <t>Pena</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -6634,7 +6634,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Gomez, Julie</t>
+          <t>Tucker, Shari</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -6644,7 +6644,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Gomez</t>
+          <t>Tucker</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -6675,7 +6675,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Smith, Susan</t>
+          <t>Page, Raymond</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Page</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -6714,7 +6714,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Bass, Joseph</t>
+          <t>Reyes, Adrian</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -6724,7 +6724,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Bass</t>
+          <t>Reyes</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -6753,7 +6753,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Ray, Tracy</t>
+          <t>Arnold, Keith</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -6763,7 +6763,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Ray</t>
+          <t>Arnold</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -6792,7 +6792,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Archer, Christine</t>
+          <t>Gilmore, Renee</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -6802,7 +6802,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Archer</t>
+          <t>Gilmore</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -6831,7 +6831,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Brown, Connor</t>
+          <t>Molina, Sarah</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Molina</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -6870,7 +6870,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Keller, Sarah</t>
+          <t>Woods, Donna</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -6880,7 +6880,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Keller</t>
+          <t>Woods</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -6909,7 +6909,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Soto, Thomas</t>
+          <t>Farley, Peggy</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -6919,7 +6919,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Soto</t>
+          <t>Farley</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -6948,7 +6948,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Thompson, Paige</t>
+          <t>Bean, Melinda</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -6958,7 +6958,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Thompson</t>
+          <t>Bean</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -6987,7 +6987,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Walls, Douglas</t>
+          <t>Campbell, Larry</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -6997,7 +6997,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Walls</t>
+          <t>Campbell</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -7026,7 +7026,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Burke, Henry</t>
+          <t>Holmes, Victor</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -7036,7 +7036,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Burke</t>
+          <t>Holmes</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -7065,7 +7065,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Burnett, Howard</t>
+          <t>Medina III, William</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -7075,7 +7075,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Burnett</t>
+          <t>Medina III</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -7106,7 +7106,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Kenneth Stephens, Mr.</t>
+          <t>Solis, Sandra</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -7116,7 +7116,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Kenneth Stephens</t>
+          <t>Solis</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -7145,7 +7145,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Jackson, Elizabeth</t>
+          <t>Richards, Henry</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -7155,7 +7155,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Richards</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -7184,7 +7184,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Mosley, Alexis</t>
+          <t>Hill, Daniel</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Mosley</t>
+          <t>Hill</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Doyle PhD, Margaret</t>
+          <t>Diaz, Jeremy</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -7233,7 +7233,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Doyle PhD</t>
+          <t>Diaz</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -7262,7 +7262,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Combs, Eric</t>
+          <t>Johnson, Jeffrey</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -7272,7 +7272,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Combs</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Booth, Richard</t>
+          <t>Newman, James</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -7311,7 +7311,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Booth</t>
+          <t>Newman</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -7340,7 +7340,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Walton, Loretta</t>
+          <t>Townsend, Stacey</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -7350,7 +7350,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Walton</t>
+          <t>Townsend</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -7379,7 +7379,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Owens, Brian</t>
+          <t>Sullivan, Wesley</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -7389,7 +7389,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Owens</t>
+          <t>Sullivan</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -7418,7 +7418,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Munoz, Joshua</t>
+          <t>Blair, Haley</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -7428,7 +7428,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Munoz</t>
+          <t>Blair</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -7457,7 +7457,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Green, Danielle</t>
+          <t>Mendoza, Traci</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -7467,7 +7467,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Mendoza</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -7496,7 +7496,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Velasquez, Jeffrey</t>
+          <t>Mueller, Heather</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -7506,7 +7506,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Velasquez</t>
+          <t>Mueller</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -7535,7 +7535,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Bowman, Katherine</t>
+          <t>Taylor, Isaiah</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -7545,7 +7545,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Bowman</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -7574,7 +7574,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Thomas, Mary</t>
+          <t>Wright, Tanya</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -7584,7 +7584,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Wright</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -7658,12 +7658,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sampson</t>
+          <t>Meyers</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Brian</t>
+          <t>Curtis</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -7681,19 +7681,19 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Brian.Sampson@fake_domain.com</t>
+          <t>Curtis.Meyers@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Molina</t>
+          <t>Richardson</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bradley</t>
+          <t>Charles</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -7711,19 +7711,19 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Bradley.Molina@fake_domain.com</t>
+          <t>Charles.Richardson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Moore</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -7741,19 +7741,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Michael.Norton@fake_domain.com</t>
+          <t>Lisa.Todd@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>Powell</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Leah</t>
+          <t>Christy</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -7771,19 +7771,19 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Leah.Joseph@fake_domain.com</t>
+          <t>Christy.Powell@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Peters</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Amberan</t>
+          <t>Davidan</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -7801,19 +7801,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Lawrence.Marshall@fake_domain.com</t>
+          <t>Carol.Peters@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hughes</t>
+          <t>Cobb</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Carrie Nathan.</t>
+          <t>John Jesse.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -7831,19 +7831,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Carrie.Hughes@fake_domain.com</t>
+          <t>John.Cobb@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Brooks</t>
+          <t>Lee</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jason </t>
+          <t xml:space="preserve">Tiffany </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -7861,19 +7861,19 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Jason.David@fake_domain.com</t>
+          <t>Tiffany.Ward@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Wilcox</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Melissa I.</t>
+          <t>Marie I.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -7891,19 +7891,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Melissa.Wilcox@fake_domain.com</t>
+          <t>Marie.Davis@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Griffin</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Linda A.</t>
+          <t>Leonard A.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -7921,19 +7921,19 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Linda.Griffin@fake_domain.com</t>
+          <t>Leonard.Smith@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Miller</t>
+          <t>Rodriguez</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Melissa</t>
+          <t>Davidnice</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -7951,19 +7951,19 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Stephanie.Miller@fake_domain.com</t>
+          <t>Gabrielle.Rodriguez@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Oliver</t>
+          <t>Stewart</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Russell</t>
+          <t>Samuel</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -7981,19 +7981,19 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Russell.Oliver@fake_domain.com</t>
+          <t>Samuel.Stewart@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Allen</t>
+          <t>Cox</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Craig</t>
+          <t>Angelica</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -8011,19 +8011,19 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Craig.Allen@fake_domain.com</t>
+          <t>Angelica.Cox@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Schroeder</t>
+          <t>Cook</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DarAlex</t>
+          <t>DarMariah</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -8041,7 +8041,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Elizabeth.Schroeder@fake_domain.com</t>
+          <t>Alejandro.Cook@fake_domain.com</t>
         </is>
       </c>
     </row>
@@ -8053,7 +8053,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>William</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -8071,19 +8071,19 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Michael.Wilson@fake_domain.com</t>
+          <t>William.Wilson@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Burnett</t>
+          <t>Montgomery</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Calvinr</t>
+          <t>Tracier</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -8101,19 +8101,19 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Calvin.Burnett@fake_domain.com</t>
+          <t>Tracie.Montgomery@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Richardson</t>
+          <t>Sanders</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Amberanette</t>
+          <t>Davidanette</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -8131,19 +8131,19 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Christopher.White@fake_domain.com</t>
+          <t>Jeffrey.Jennings@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Burgess DVM</t>
+          <t>Evans</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Julia</t>
+          <t>Amanda</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -8161,19 +8161,19 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Danielle.Burgess.DVM@fake_domain.com</t>
+          <t>Stephen.Evans@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Lopez</t>
+          <t>Taylor</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Joshua Cheryl</t>
+          <t>Christopher James</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -8191,19 +8191,19 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Joshua.Lopez@fake_domain.com </t>
+          <t xml:space="preserve">Christopher.Taylor@fake_domain.com </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Barker</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ashley</t>
+          <t>Karen</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -8221,19 +8221,19 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Ashley.Barker@fake_domain.com</t>
+          <t>Karen.Williams@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Cooper</t>
+          <t>Ramirez</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Deborah</t>
+          <t>Jennifer</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -8251,19 +8251,19 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Deborah.Cooper@fake_domain.com</t>
+          <t>Jennifer.Ramirez@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Alvarado</t>
+          <t>Adams</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Rebecca Nathan.</t>
+          <t>Dale Jesse.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -8281,19 +8281,19 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Rebecca.Alvarado@fake_domain.com</t>
+          <t>Dale.Adams@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Wiley</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Adrianlas R.</t>
+          <t>Miguellas R.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -8311,19 +8311,19 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Michael.Lopez@fake_domain.com</t>
+          <t>Brandon.Hernandez@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Wiley</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve">James D. </t>
+          <t xml:space="preserve">Julie D. </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -8341,19 +8341,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>James.Shannon@fake_domain.com</t>
+          <t>Julie.Moran@fake_domain.com</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Natasha Alexander MD</t>
+          <t>Hansen</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Dr.</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -8371,7 +8371,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Dr.Natasha.Alexander.MD@fake_domain.com</t>
+          <t>Lucas.Hansen@fake_domain.com</t>
         </is>
       </c>
     </row>

</xml_diff>